<commit_message>
add screen for wroking gps and glonass
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>1575,42 МГц</t>
   </si>
@@ -71,6 +71,24 @@
   </si>
   <si>
     <t>5249969.01</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>-70</t>
+  </si>
+  <si>
+    <t>GPS status</t>
+  </si>
+  <si>
+    <t>GLONASS status</t>
+  </si>
+  <si>
+    <t>on</t>
   </si>
 </sst>
 </file>
@@ -87,7 +105,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -110,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -133,23 +151,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -454,230 +494,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.36328125" customWidth="1"/>
-    <col min="10" max="10" width="7.26953125" customWidth="1"/>
-    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.36328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="7.26953125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1796875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="L1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="1">
         <v>0.95</v>
       </c>
-      <c r="J2" s="4">
-        <v>43405</v>
-      </c>
-      <c r="K2" s="5">
-        <v>43160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>